<commit_message>
E pushes data but its temperamental
</commit_message>
<xml_diff>
--- a/data/phenology/phenocam_pics/QHI_phenocams_all_final.xlsx
+++ b/data/phenology/phenocam_pics/QHI_phenocams_all_final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericazaja/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericazaja/Desktop/Github_repos.tmp/GardenHub/data/phenology/phenocam_pics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FED8E22-B6B2-BE4F-B947-1C657DD3136F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27245CA-19FF-DC4C-8D59-0FFA08841EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - phenocams_19012022 co" sheetId="1" r:id="rId1"/>
@@ -778,7 +778,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -837,7 +837,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -898,18 +897,14 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="6" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2073,8 +2068,8 @@
   </sheetPr>
   <dimension ref="A1:BB44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="185" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L3" zoomScale="185" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2097,10 +2092,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="47" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="46" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -2112,19 +2107,19 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="47" t="s">
         <v>159</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="47" t="s">
         <v>160</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="47" t="s">
         <v>161</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="I1" s="47" t="s">
         <v>162</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="47" t="s">
         <v>163</v>
       </c>
       <c r="K1" s="2" t="s">
@@ -2148,13 +2143,13 @@
       <c r="Q1" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="R1" s="53" t="s">
+      <c r="R1" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="S1" s="53" t="s">
+      <c r="S1" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="T1" s="53" t="s">
+      <c r="T1" s="47" t="s">
         <v>166</v>
       </c>
     </row>
@@ -2213,7 +2208,7 @@
       <c r="R2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="47">
+      <c r="S2" s="48">
         <v>43671</v>
       </c>
       <c r="T2" s="8" t="s">
@@ -2461,7 +2456,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="19"/>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="48" t="s">
         <v>29</v>
       </c>
       <c r="F7" s="18" t="s">
@@ -2500,7 +2495,7 @@
       <c r="Q7" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="R7" s="22">
+      <c r="R7" s="48">
         <v>43275</v>
       </c>
       <c r="S7" s="20" t="s">
@@ -2624,7 +2619,7 @@
       <c r="Q9" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="R9" s="22">
+      <c r="R9" s="48">
         <v>43276</v>
       </c>
       <c r="S9" s="20" t="s">
@@ -2686,7 +2681,7 @@
       <c r="Q10" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="R10" s="22">
+      <c r="R10" s="48">
         <v>43277</v>
       </c>
       <c r="S10" s="20" t="s">
@@ -2808,64 +2803,64 @@
       <c r="Q12" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="R12" s="22">
+      <c r="R12" s="48">
         <v>43275</v>
       </c>
-      <c r="S12" s="22">
+      <c r="S12" s="48">
         <v>43328</v>
       </c>
-      <c r="T12" s="22">
+      <c r="T12" s="48">
         <v>43354</v>
       </c>
     </row>
-    <row r="13" spans="1:20" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
+    <row r="13" spans="1:20" s="27" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="23">
         <v>2017</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="25" t="s">
+      <c r="D13" s="25"/>
+      <c r="E13" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="J13" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="25" t="s">
+      <c r="H13" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="L13" s="25" t="s">
+      <c r="L13" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="M13" s="25" t="s">
+      <c r="M13" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="N13" s="25" t="s">
+      <c r="N13" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="O13" s="25" t="s">
+      <c r="O13" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="P13" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q13" s="27" t="s">
+      <c r="P13" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q13" s="26" t="s">
         <v>153</v>
       </c>
       <c r="R13" s="48">
@@ -2878,56 +2873,56 @@
         <v>42982</v>
       </c>
     </row>
-    <row r="14" spans="1:20" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+    <row r="14" spans="1:20" s="27" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="23">
         <v>2017</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="E14" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="J14" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="K14" s="25" t="s">
+      <c r="E14" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="L14" s="25" t="s">
+      <c r="L14" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="M14" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="N14" s="25" t="s">
+      <c r="M14" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="N14" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="O14" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="P14" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q14" s="27" t="s">
+      <c r="O14" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="P14" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q14" s="26" t="s">
         <v>153</v>
       </c>
       <c r="R14" s="48">
@@ -2936,60 +2931,60 @@
       <c r="S14" s="48">
         <v>42956</v>
       </c>
-      <c r="T14" s="27" t="s">
+      <c r="T14" s="26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
+    <row r="15" spans="1:20" s="27" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="23">
         <v>2017</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="H15" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="J15" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="K15" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="L15" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="M15" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="N15" s="25" t="s">
+      <c r="H15" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="M15" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="N15" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="O15" s="25" t="s">
+      <c r="O15" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="P15" s="25" t="s">
+      <c r="P15" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="Q15" s="27" t="s">
+      <c r="Q15" s="26" t="s">
         <v>154</v>
       </c>
       <c r="R15" s="48">
@@ -3002,118 +2997,118 @@
         <v>42981</v>
       </c>
     </row>
-    <row r="16" spans="1:20" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
+    <row r="16" spans="1:20" s="27" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="23">
         <v>2017</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="E16" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="25" t="s">
+      <c r="E16" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="H16" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="J16" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="K16" s="25" t="s">
+      <c r="H16" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="L16" s="25" t="s">
+      <c r="L16" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="M16" s="25" t="s">
+      <c r="M16" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="N16" s="25" t="s">
+      <c r="N16" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="O16" s="25" t="s">
+      <c r="O16" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="P16" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q16" s="27" t="s">
+      <c r="P16" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q16" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="R16" s="27" t="s">
+      <c r="R16" s="26" t="s">
         <v>13</v>
       </c>
       <c r="S16" s="48">
         <v>42952</v>
       </c>
-      <c r="T16" s="27" t="s">
+      <c r="T16" s="26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
+    <row r="17" spans="1:20" s="27" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="23">
         <v>2017</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="G17" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="H17" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="J17" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="K17" s="25" t="s">
+      <c r="H17" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="L17" s="25" t="s">
+      <c r="L17" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="M17" s="25" t="s">
+      <c r="M17" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="N17" s="25" t="s">
+      <c r="N17" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="O17" s="25" t="s">
+      <c r="O17" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="P17" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q17" s="27" t="s">
+      <c r="P17" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q17" s="26" t="s">
         <v>153</v>
       </c>
       <c r="R17" s="48">
@@ -3122,60 +3117,60 @@
       <c r="S17" s="48">
         <v>42956</v>
       </c>
-      <c r="T17" s="27" t="s">
+      <c r="T17" s="26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:20" s="28" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="23" t="s">
+    <row r="18" spans="1:20" s="27" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="23">
         <v>2017</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="F18" s="25" t="s">
+      <c r="F18" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="G18" s="25" t="s">
+      <c r="G18" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="H18" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="J18" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="K18" s="25" t="s">
+      <c r="H18" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="L18" s="25" t="s">
+      <c r="L18" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M18" s="25" t="s">
+      <c r="M18" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="N18" s="25" t="s">
+      <c r="N18" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="O18" s="25" t="s">
+      <c r="O18" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="P18" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q18" s="27" t="s">
+      <c r="P18" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q18" s="26" t="s">
         <v>154</v>
       </c>
       <c r="R18" s="48">
@@ -3188,1613 +3183,1613 @@
         <v>42971</v>
       </c>
     </row>
-    <row r="19" spans="1:20" s="33" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="29" t="s">
+    <row r="19" spans="1:20" s="32" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="30">
+      <c r="B19" s="29">
         <v>2016</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="J19" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="K19" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="L19" s="31" t="s">
+      <c r="E19" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="K19" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="L19" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="M19" s="31" t="s">
+      <c r="M19" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="N19" s="31" t="s">
+      <c r="N19" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="O19" s="31" t="s">
+      <c r="O19" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="P19" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q19" s="32" t="s">
+      <c r="P19" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q19" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="R19" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="S19" s="49">
+      <c r="R19" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="S19" s="48">
         <v>42580</v>
       </c>
-      <c r="T19" s="32" t="s">
+      <c r="T19" s="31" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:20" s="33" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="29" t="s">
+    <row r="20" spans="1:20" s="32" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="30">
+      <c r="B20" s="29">
         <v>2016</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="E20" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="J20" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="K20" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="L20" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="M20" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="N20" s="31" t="s">
+      <c r="E20" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="L20" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="M20" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="N20" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="O20" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="P20" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q20" s="32" t="s">
+      <c r="O20" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="P20" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q20" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="R20" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="S20" s="49">
+      <c r="R20" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="S20" s="48">
         <v>42580</v>
       </c>
-      <c r="T20" s="32" t="s">
+      <c r="T20" s="31" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="33" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="29" t="s">
+    <row r="21" spans="1:20" s="32" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="30">
+      <c r="B21" s="29">
         <v>2016</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="E21" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="J21" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="K21" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="L21" s="31" t="s">
+      <c r="E21" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="M21" s="31" t="s">
+      <c r="M21" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="N21" s="31" t="s">
+      <c r="N21" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="O21" s="31" t="s">
+      <c r="O21" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="P21" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q21" s="32" t="s">
+      <c r="P21" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q21" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="R21" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="S21" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="T21" s="32" t="s">
+      <c r="R21" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="S21" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="T21" s="31" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:20" s="33" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="29" t="s">
+    <row r="22" spans="1:20" s="32" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="30">
+      <c r="B22" s="29">
         <v>2016</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="E22" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="31" t="s">
+      <c r="E22" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="G22" s="31" t="s">
+      <c r="G22" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="H22" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="I22" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="J22" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="K22" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="L22" s="31" t="s">
+      <c r="H22" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="L22" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="M22" s="31" t="s">
+      <c r="M22" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="N22" s="31" t="s">
+      <c r="N22" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="O22" s="31" t="s">
+      <c r="O22" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="P22" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q22" s="32" t="s">
+      <c r="P22" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q22" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="R22" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="S22" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="T22" s="49">
+      <c r="R22" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="S22" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="T22" s="48">
         <v>42610</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="33" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="29" t="s">
+    <row r="23" spans="1:20" s="32" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="30">
+      <c r="B23" s="29">
         <v>2016</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="E23" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="J23" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="K23" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="L23" s="31" t="s">
+      <c r="E23" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="K23" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="L23" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="M23" s="31" t="s">
+      <c r="M23" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="N23" s="31" t="s">
+      <c r="N23" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="O23" s="31" t="s">
+      <c r="O23" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="P23" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q23" s="32" t="s">
+      <c r="P23" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q23" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="R23" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="S23" s="49">
+      <c r="R23" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="S23" s="48">
         <v>42580</v>
       </c>
-      <c r="T23" s="49">
+      <c r="T23" s="48">
         <v>42608</v>
       </c>
     </row>
-    <row r="24" spans="1:20" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="34" t="s">
+    <row r="24" spans="1:20" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="35">
+      <c r="B24" s="34">
         <v>2016</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="36" t="s">
+      <c r="D24" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="E24" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I24" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J24" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K24" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L24" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M24" s="36" t="s">
+      <c r="E24" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K24" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L24" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M24" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="N24" s="36" t="s">
+      <c r="N24" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="O24" s="36" t="s">
+      <c r="O24" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="P24" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q24" s="37" t="s">
+      <c r="P24" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q24" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="R24" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="S24" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="T24" s="51">
+      <c r="R24" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="S24" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="T24" s="48">
         <v>44800</v>
       </c>
     </row>
-    <row r="25" spans="1:20" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="34" t="s">
+    <row r="25" spans="1:20" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="35">
+      <c r="B25" s="34">
         <v>2022</v>
       </c>
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="39"/>
-      <c r="E25" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I25" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J25" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K25" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L25" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M25" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N25" s="36" t="s">
+      <c r="D25" s="38"/>
+      <c r="E25" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K25" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L25" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M25" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N25" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="O25" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P25" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q25" s="40" t="s">
+      <c r="O25" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P25" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q25" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="R25" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S25" s="50">
+      <c r="R25" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S25" s="48">
         <v>44743</v>
       </c>
-      <c r="T25" s="41" t="s">
+      <c r="T25" s="40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="34" t="s">
+    <row r="26" spans="1:20" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="35">
+      <c r="B26" s="34">
         <v>2022</v>
       </c>
-      <c r="C26" s="36" t="s">
+      <c r="C26" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="39"/>
-      <c r="E26" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I26" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J26" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K26" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L26" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M26" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N26" s="42" t="s">
+      <c r="D26" s="38"/>
+      <c r="E26" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J26" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K26" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L26" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M26" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N26" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="O26" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P26" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q26" s="40" t="s">
+      <c r="O26" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P26" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q26" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="R26" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S26" s="50">
+      <c r="R26" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S26" s="48">
         <v>44743</v>
       </c>
-      <c r="T26" s="41" t="s">
+      <c r="T26" s="40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:20" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="34" t="s">
+    <row r="27" spans="1:20" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="35">
+      <c r="B27" s="34">
         <v>2022</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="39"/>
-      <c r="E27" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I27" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J27" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K27" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L27" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M27" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N27" s="36" t="s">
+      <c r="D27" s="38"/>
+      <c r="E27" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J27" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K27" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L27" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M27" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N27" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="O27" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P27" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q27" s="43" t="s">
+      <c r="O27" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P27" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q27" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="R27" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S27" s="50">
+      <c r="R27" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S27" s="48">
         <v>44743</v>
       </c>
-      <c r="T27" s="41" t="s">
+      <c r="T27" s="40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:20" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="34" t="s">
+    <row r="28" spans="1:20" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="B28" s="35">
+      <c r="B28" s="34">
         <v>2022</v>
       </c>
-      <c r="C28" s="36" t="s">
+      <c r="C28" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="39"/>
-      <c r="E28" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H28" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I28" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J28" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K28" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L28" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M28" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N28" s="36" t="s">
+      <c r="D28" s="38"/>
+      <c r="E28" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I28" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J28" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K28" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L28" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M28" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N28" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="O28" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P28" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q28" s="43" t="s">
+      <c r="O28" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P28" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q28" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="R28" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S28" s="50">
+      <c r="R28" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S28" s="48">
         <v>44743</v>
       </c>
-      <c r="T28" s="41" t="s">
+      <c r="T28" s="40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:20" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="34" t="s">
+    <row r="29" spans="1:20" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="35">
+      <c r="B29" s="34">
         <v>2022</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="39"/>
-      <c r="E29" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H29" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I29" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J29" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K29" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L29" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M29" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N29" s="36" t="s">
+      <c r="D29" s="38"/>
+      <c r="E29" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J29" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K29" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L29" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M29" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N29" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="O29" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P29" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q29" s="40" t="s">
+      <c r="O29" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P29" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q29" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="R29" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S29" s="50">
+      <c r="R29" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S29" s="48">
         <v>44773</v>
       </c>
-      <c r="T29" s="41" t="s">
+      <c r="T29" s="40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:20" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="34" t="s">
+    <row r="30" spans="1:20" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="35">
+      <c r="B30" s="34">
         <v>2022</v>
       </c>
-      <c r="C30" s="36" t="s">
+      <c r="C30" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="39"/>
-      <c r="E30" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H30" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I30" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J30" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K30" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L30" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M30" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N30" s="36" t="s">
+      <c r="D30" s="38"/>
+      <c r="E30" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K30" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L30" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M30" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N30" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="O30" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P30" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q30" s="43" t="s">
+      <c r="O30" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P30" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q30" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="R30" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S30" s="50">
+      <c r="R30" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S30" s="48">
         <v>44762</v>
       </c>
-      <c r="T30" s="41" t="s">
+      <c r="T30" s="40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:20" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="34" t="s">
+    <row r="31" spans="1:20" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="B31" s="35">
+      <c r="B31" s="34">
         <v>2022</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="C31" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="39"/>
-      <c r="E31" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H31" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I31" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J31" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K31" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L31" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M31" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N31" s="36" t="s">
+      <c r="D31" s="38"/>
+      <c r="E31" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I31" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J31" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K31" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L31" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M31" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N31" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="O31" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P31" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q31" s="43" t="s">
+      <c r="O31" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P31" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q31" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="R31" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S31" s="50">
+      <c r="R31" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S31" s="48">
         <v>44770</v>
       </c>
-      <c r="T31" s="41" t="s">
+      <c r="T31" s="40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:20" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="34" t="s">
+    <row r="32" spans="1:20" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B32" s="35">
+      <c r="B32" s="34">
         <v>2022</v>
       </c>
-      <c r="C32" s="36" t="s">
+      <c r="C32" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="39"/>
-      <c r="E32" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H32" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I32" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J32" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K32" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L32" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M32" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N32" s="36" t="s">
+      <c r="D32" s="38"/>
+      <c r="E32" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K32" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L32" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M32" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N32" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="O32" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P32" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q32" s="43" t="s">
+      <c r="O32" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P32" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q32" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="R32" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S32" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="T32" s="41" t="s">
+      <c r="R32" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S32" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="T32" s="40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:54" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="34" t="s">
+    <row r="33" spans="1:54" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="B33" s="35">
+      <c r="B33" s="34">
         <v>2022</v>
       </c>
-      <c r="C33" s="36" t="s">
+      <c r="C33" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="39"/>
-      <c r="E33" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I33" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J33" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K33" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L33" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M33" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N33" s="36" t="s">
+      <c r="D33" s="38"/>
+      <c r="E33" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I33" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J33" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K33" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L33" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M33" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N33" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="O33" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P33" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q33" s="43" t="s">
+      <c r="O33" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P33" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q33" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="R33" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S33" s="50">
+      <c r="R33" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S33" s="48">
         <v>44764</v>
       </c>
-      <c r="T33" s="41" t="s">
+      <c r="T33" s="40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:54" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="34" t="s">
+    <row r="34" spans="1:54" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="B34" s="35">
+      <c r="B34" s="34">
         <v>2022</v>
       </c>
-      <c r="C34" s="36" t="s">
+      <c r="C34" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="39"/>
-      <c r="E34" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H34" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I34" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J34" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K34" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L34" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M34" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N34" s="36" t="s">
+      <c r="D34" s="38"/>
+      <c r="E34" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I34" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J34" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K34" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L34" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M34" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N34" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="O34" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P34" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q34" s="40" t="s">
+      <c r="O34" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P34" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q34" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="R34" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S34" s="50">
+      <c r="R34" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S34" s="48">
         <v>44768</v>
       </c>
-      <c r="T34" s="41" t="s">
+      <c r="T34" s="40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:54" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="34" t="s">
+    <row r="35" spans="1:54" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="B35" s="35">
+      <c r="B35" s="34">
         <v>2022</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="39"/>
-      <c r="E35" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I35" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J35" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K35" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L35" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M35" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N35" s="36" t="s">
+      <c r="D35" s="38"/>
+      <c r="E35" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I35" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J35" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K35" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L35" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M35" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N35" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="O35" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P35" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q35" s="43" t="s">
+      <c r="O35" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P35" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q35" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="R35" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S35" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="T35" s="41" t="s">
+      <c r="R35" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S35" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="T35" s="40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:54" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="34" t="s">
+    <row r="36" spans="1:54" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="B36" s="35">
+      <c r="B36" s="34">
         <v>2022</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="C36" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="39"/>
-      <c r="E36" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H36" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I36" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J36" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K36" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L36" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M36" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N36" s="36" t="s">
+      <c r="D36" s="38"/>
+      <c r="E36" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I36" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J36" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L36" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M36" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N36" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="O36" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P36" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q36" s="43" t="s">
+      <c r="O36" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P36" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q36" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="R36" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S36" s="50">
+      <c r="R36" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S36" s="48">
         <v>44769</v>
       </c>
-      <c r="T36" s="41" t="s">
+      <c r="T36" s="40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:54" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="34" t="s">
+    <row r="37" spans="1:54" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="B37" s="35">
+      <c r="B37" s="34">
         <v>2022</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="39"/>
-      <c r="E37" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H37" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I37" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J37" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K37" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L37" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M37" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N37" s="36" t="s">
+      <c r="D37" s="38"/>
+      <c r="E37" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I37" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J37" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K37" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L37" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M37" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N37" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="O37" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P37" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q37" s="40" t="s">
+      <c r="O37" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P37" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q37" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="R37" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S37" s="50">
+      <c r="R37" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S37" s="48">
         <v>44776</v>
       </c>
-      <c r="T37" s="41" t="s">
+      <c r="T37" s="40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:54" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="34" t="s">
+    <row r="38" spans="1:54" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="35">
+      <c r="B38" s="34">
         <v>2022</v>
       </c>
-      <c r="C38" s="36" t="s">
+      <c r="C38" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="39"/>
-      <c r="E38" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H38" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I38" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J38" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K38" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L38" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M38" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N38" s="36" t="s">
+      <c r="D38" s="38"/>
+      <c r="E38" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I38" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J38" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K38" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L38" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M38" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N38" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="O38" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P38" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q38" s="43" t="s">
+      <c r="O38" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P38" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q38" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="R38" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S38" s="50">
+      <c r="R38" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S38" s="48">
         <v>44771</v>
       </c>
-      <c r="T38" s="41" t="s">
+      <c r="T38" s="40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:54" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="34" t="s">
+    <row r="39" spans="1:54" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="B39" s="35">
+      <c r="B39" s="34">
         <v>2022</v>
       </c>
-      <c r="C39" s="36" t="s">
+      <c r="C39" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="39"/>
-      <c r="E39" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G39" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I39" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J39" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K39" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L39" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M39" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N39" s="36" t="s">
+      <c r="D39" s="38"/>
+      <c r="E39" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I39" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J39" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K39" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L39" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M39" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N39" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="O39" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P39" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q39" s="43" t="s">
+      <c r="O39" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P39" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q39" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="R39" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S39" s="50">
+      <c r="R39" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S39" s="48">
         <v>44776</v>
       </c>
-      <c r="T39" s="41" t="s">
+      <c r="T39" s="40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:54" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="34" t="s">
+    <row r="40" spans="1:54" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="B40" s="35">
+      <c r="B40" s="34">
         <v>2022</v>
       </c>
-      <c r="C40" s="36" t="s">
+      <c r="C40" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D40" s="39"/>
-      <c r="E40" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G40" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H40" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I40" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J40" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K40" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L40" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M40" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N40" s="36" t="s">
+      <c r="D40" s="38"/>
+      <c r="E40" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I40" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J40" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K40" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L40" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M40" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N40" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="O40" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P40" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q40" s="43" t="s">
+      <c r="O40" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P40" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q40" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="R40" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S40" s="50">
+      <c r="R40" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S40" s="48">
         <v>44778</v>
       </c>
-      <c r="T40" s="41" t="s">
+      <c r="T40" s="40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:54" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="34" t="s">
+    <row r="41" spans="1:54" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="B41" s="35">
+      <c r="B41" s="34">
         <v>2022</v>
       </c>
-      <c r="C41" s="36" t="s">
+      <c r="C41" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="39"/>
-      <c r="E41" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F41" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G41" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H41" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I41" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J41" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K41" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L41" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M41" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N41" s="36" t="s">
+      <c r="D41" s="38"/>
+      <c r="E41" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I41" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J41" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K41" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L41" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M41" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N41" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="O41" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P41" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q41" s="43" t="s">
+      <c r="O41" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P41" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q41" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="R41" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S41" s="50">
+      <c r="R41" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S41" s="48">
         <v>44771</v>
       </c>
-      <c r="T41" s="41" t="s">
+      <c r="T41" s="40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:54" s="44" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="34" t="s">
+    <row r="42" spans="1:54" s="43" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="B42" s="37">
+      <c r="B42" s="36">
         <v>2022</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C42" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E42" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="F42" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="G42" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="H42" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="I42" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="J42" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="K42" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="L42" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="M42" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="N42" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="O42" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="P42" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q42" s="40" t="s">
+      <c r="E42" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="I42" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="J42" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="K42" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="L42" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="M42" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="N42" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="O42" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="P42" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q42" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="R42" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S42" s="50">
+      <c r="R42" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S42" s="48">
         <v>44769</v>
       </c>
-      <c r="T42" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="U42" s="43"/>
-      <c r="V42" s="43"/>
-      <c r="W42" s="43"/>
-      <c r="X42" s="43"/>
-      <c r="Y42" s="43"/>
-      <c r="Z42" s="43"/>
-      <c r="AA42" s="43"/>
-      <c r="AB42" s="43"/>
-      <c r="AC42" s="43"/>
-      <c r="AD42" s="43"/>
-      <c r="AE42" s="45"/>
-      <c r="AF42" s="46"/>
-      <c r="AG42" s="46"/>
-      <c r="AH42" s="46"/>
-      <c r="AI42" s="46"/>
-      <c r="AJ42" s="46"/>
-      <c r="AK42" s="43"/>
-      <c r="AL42" s="43"/>
-      <c r="AM42" s="43"/>
-      <c r="AN42" s="43"/>
-      <c r="AO42" s="43"/>
-      <c r="AP42" s="43"/>
-      <c r="AQ42" s="43"/>
-      <c r="AR42" s="43"/>
-      <c r="AS42" s="43"/>
-      <c r="AT42" s="43"/>
-      <c r="AU42" s="43"/>
-      <c r="AV42" s="43"/>
-      <c r="AW42" s="43"/>
-      <c r="AX42" s="43"/>
-      <c r="AY42" s="43"/>
-      <c r="AZ42" s="46"/>
-      <c r="BA42" s="46"/>
-      <c r="BB42" s="46"/>
+      <c r="T42" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="U42" s="42"/>
+      <c r="V42" s="42"/>
+      <c r="W42" s="42"/>
+      <c r="X42" s="42"/>
+      <c r="Y42" s="42"/>
+      <c r="Z42" s="42"/>
+      <c r="AA42" s="42"/>
+      <c r="AB42" s="42"/>
+      <c r="AC42" s="42"/>
+      <c r="AD42" s="42"/>
+      <c r="AE42" s="44"/>
+      <c r="AF42" s="45"/>
+      <c r="AG42" s="45"/>
+      <c r="AH42" s="45"/>
+      <c r="AI42" s="45"/>
+      <c r="AJ42" s="45"/>
+      <c r="AK42" s="42"/>
+      <c r="AL42" s="42"/>
+      <c r="AM42" s="42"/>
+      <c r="AN42" s="42"/>
+      <c r="AO42" s="42"/>
+      <c r="AP42" s="42"/>
+      <c r="AQ42" s="42"/>
+      <c r="AR42" s="42"/>
+      <c r="AS42" s="42"/>
+      <c r="AT42" s="42"/>
+      <c r="AU42" s="42"/>
+      <c r="AV42" s="42"/>
+      <c r="AW42" s="42"/>
+      <c r="AX42" s="42"/>
+      <c r="AY42" s="42"/>
+      <c r="AZ42" s="45"/>
+      <c r="BA42" s="45"/>
+      <c r="BB42" s="45"/>
     </row>
-    <row r="43" spans="1:54" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="34" t="s">
+    <row r="43" spans="1:54" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="B43" s="35">
+      <c r="B43" s="34">
         <v>2022</v>
       </c>
-      <c r="C43" s="36" t="s">
+      <c r="C43" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="39"/>
-      <c r="E43" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F43" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G43" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H43" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I43" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J43" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K43" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L43" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M43" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N43" s="36" t="s">
+      <c r="D43" s="38"/>
+      <c r="E43" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I43" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J43" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K43" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L43" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M43" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N43" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="O43" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P43" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q43" s="40" t="s">
+      <c r="O43" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P43" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q43" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="R43" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S43" s="50">
+      <c r="R43" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S43" s="48">
         <v>44773</v>
       </c>
-      <c r="T43" s="41" t="s">
+      <c r="T43" s="40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:54" s="38" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="34" t="s">
+    <row r="44" spans="1:54" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="B44" s="35">
+      <c r="B44" s="34">
         <v>2022</v>
       </c>
-      <c r="C44" s="36" t="s">
+      <c r="C44" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D44" s="39"/>
-      <c r="E44" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F44" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H44" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I44" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="J44" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K44" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="L44" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M44" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="N44" s="36" t="s">
+      <c r="D44" s="38"/>
+      <c r="E44" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I44" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J44" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="K44" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L44" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="M44" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="N44" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="O44" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="P44" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q44" s="40" t="s">
+      <c r="O44" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="P44" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q44" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="R44" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="S44" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="T44" s="41" t="s">
+      <c r="R44" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="S44" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="T44" s="40" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="X42 V42 Z42 AB42 AD42 AF42 AH42 AJ42 AL42">
+  <conditionalFormatting sqref="V42 X42 Z42 AB42 AD42 AF42 AH42 AJ42 AL42">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="formula" val="1"/>

</xml_diff>

<commit_message>
E adds note on temp data being soil
</commit_message>
<xml_diff>
--- a/data/phenology/phenocam_pics/QHI_phenocams_all_final.xlsx
+++ b/data/phenology/phenocam_pics/QHI_phenocams_all_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericazaja/Desktop/Github_repos.tmp/GardenHub/data/phenology/phenocam_pics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F19E1EF-8D8A-E645-BA66-11EF7621E950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF9E09C-0458-DC44-B98D-A78DC7CCA7F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="5580" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - phenocams_19012022 co" sheetId="1" r:id="rId1"/>
@@ -34,24 +34,6 @@
     <t>plant_first_vis</t>
   </si>
   <si>
-    <t>bud_burst</t>
-  </si>
-  <si>
-    <t>green50</t>
-  </si>
-  <si>
-    <t>green100</t>
-  </si>
-  <si>
-    <t>first_yellow</t>
-  </si>
-  <si>
-    <t>yellow50</t>
-  </si>
-  <si>
-    <t>yellow100</t>
-  </si>
-  <si>
     <t>QHI_1</t>
   </si>
   <si>
@@ -521,6 +503,24 @@
   </si>
   <si>
     <t>Salix_last_yellow</t>
+  </si>
+  <si>
+    <t>First_leaf_bud_burst</t>
+  </si>
+  <si>
+    <t>Half_leaves_green</t>
+  </si>
+  <si>
+    <t>All_leaves_green</t>
+  </si>
+  <si>
+    <t>First_leaf_yellow</t>
+  </si>
+  <si>
+    <t>Half_leaves_yellow</t>
+  </si>
+  <si>
+    <t>All_leaves_yellow</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -916,9 +916,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2114,8 +2111,8 @@
   </sheetPr>
   <dimension ref="A1:AX44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M1" zoomScale="185" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="185" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2130,7 +2127,7 @@
     <col min="8" max="9" width="14.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="15.33203125" style="1" customWidth="1"/>
     <col min="11" max="13" width="10" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5" style="57" customWidth="1"/>
+    <col min="14" max="14" width="10.5" style="56" customWidth="1"/>
     <col min="15" max="16" width="10" style="1" customWidth="1"/>
     <col min="17" max="17" width="9.83203125" style="3" customWidth="1"/>
     <col min="18" max="20" width="10.5" style="3" customWidth="1"/>
@@ -2139,7 +2136,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="46" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B1" s="45" t="s">
         <v>0</v>
@@ -2154,160 +2151,160 @@
         <v>3</v>
       </c>
       <c r="F1" s="46" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="I1" s="46" t="s">
+        <v>156</v>
+      </c>
+      <c r="J1" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="R1" s="46" t="s">
+        <v>158</v>
+      </c>
+      <c r="S1" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="T1" s="46" t="s">
         <v>160</v>
-      </c>
-      <c r="H1" s="46" t="s">
-        <v>161</v>
-      </c>
-      <c r="I1" s="46" t="s">
-        <v>162</v>
-      </c>
-      <c r="J1" s="46" t="s">
-        <v>163</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="49" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="R1" s="46" t="s">
-        <v>164</v>
-      </c>
-      <c r="S1" s="46" t="s">
-        <v>165</v>
-      </c>
-      <c r="T1" s="46" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B2" s="6">
         <v>2019</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="50" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="N2" s="49" t="s">
+        <v>9</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="R2" s="8"/>
-      <c r="S2" s="58">
+      <c r="S2" s="57">
         <v>43671</v>
       </c>
       <c r="T2" s="48"/>
     </row>
     <row r="3" spans="1:20" s="9" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B3" s="11">
         <v>2019</v>
       </c>
       <c r="C3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>17</v>
-      </c>
       <c r="E3" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" s="51" t="s">
-        <v>18</v>
+        <v>7</v>
+      </c>
+      <c r="N3" s="50" t="s">
+        <v>12</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P3" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
@@ -2315,53 +2312,53 @@
     </row>
     <row r="4" spans="1:20" s="9" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B4" s="11">
         <v>2019</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="51" t="s">
-        <v>20</v>
+        <v>7</v>
+      </c>
+      <c r="N4" s="50" t="s">
+        <v>14</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q4" s="14" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="R4" s="15"/>
       <c r="S4" s="15"/>
@@ -2369,7 +2366,7 @@
     </row>
     <row r="5" spans="1:20" s="9" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="10" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B5" s="11">
         <v>2019</v>
@@ -2377,43 +2374,43 @@
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" s="51" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="N5" s="50" t="s">
+        <v>17</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q5" s="14" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="R5" s="15"/>
       <c r="S5" s="15"/>
@@ -2421,55 +2418,55 @@
     </row>
     <row r="6" spans="1:20" s="9" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B6" s="11">
         <v>2019</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="N6" s="51" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="N6" s="50" t="s">
+        <v>22</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
@@ -2477,53 +2474,53 @@
     </row>
     <row r="7" spans="1:20" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B7" s="17">
         <v>2018</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="47" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L7" s="18" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M7" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="N7" s="47" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="O7" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P7" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q7" s="20" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="R7" s="48">
         <v>43275</v>
@@ -2533,55 +2530,55 @@
     </row>
     <row r="8" spans="1:20" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B8" s="17">
         <v>2018</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="L8" s="18" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="M8" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="N8" s="47" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="O8" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P8" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q8" s="20" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="R8" s="20"/>
       <c r="S8" s="20"/>
@@ -2589,55 +2586,55 @@
     </row>
     <row r="9" spans="1:20" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B9" s="17">
         <v>2018</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="M9" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="N9" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="L9" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="M9" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="N9" s="47" t="s">
-        <v>47</v>
-      </c>
       <c r="O9" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P9" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q9" s="20" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="R9" s="47">
         <v>43276</v>
@@ -2647,55 +2644,55 @@
     </row>
     <row r="10" spans="1:20" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B10" s="17">
         <v>2018</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D10" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="M10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="N10" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="O10" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="P10" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="K10" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="L10" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="M10" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="N10" s="47" t="s">
-        <v>13</v>
-      </c>
-      <c r="O10" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="P10" s="18" t="s">
-        <v>54</v>
-      </c>
       <c r="Q10" s="20" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="R10" s="47">
         <v>43277</v>
@@ -2705,53 +2702,53 @@
     </row>
     <row r="11" spans="1:20" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B11" s="17">
         <v>2018</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="L11" s="18" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="M11" s="18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="N11" s="47" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="O11" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P11" s="18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q11" s="20" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="R11" s="20"/>
       <c r="S11" s="20"/>
@@ -2759,55 +2756,55 @@
     </row>
     <row r="12" spans="1:20" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B12" s="17">
         <v>2018</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D12" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="L12" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="M12" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="18" t="s">
+      <c r="N12" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="O12" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="P12" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="I12" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="J12" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="K12" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="L12" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="M12" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="N12" s="47" t="s">
-        <v>13</v>
-      </c>
-      <c r="O12" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="P12" s="18" t="s">
-        <v>64</v>
-      </c>
       <c r="Q12" s="20" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="R12" s="47">
         <v>43275</v>
@@ -2821,53 +2818,53 @@
     </row>
     <row r="13" spans="1:20" s="27" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B13" s="23">
         <v>2017</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F13" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M13" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="N13" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="O13" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="J13" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="L13" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="M13" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="N13" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="O13" s="24" t="s">
-        <v>71</v>
-      </c>
       <c r="P13" s="24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q13" s="26" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="R13" s="47">
         <v>42903</v>
@@ -2881,55 +2878,55 @@
     </row>
     <row r="14" spans="1:20" s="27" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B14" s="23">
         <v>2017</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K14" s="24" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="L14" s="24" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="M14" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="N14" s="52" t="s">
-        <v>70</v>
+        <v>7</v>
+      </c>
+      <c r="N14" s="51" t="s">
+        <v>64</v>
       </c>
       <c r="O14" s="24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P14" s="24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q14" s="26" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="R14" s="47">
         <v>42897</v>
@@ -2941,55 +2938,55 @@
     </row>
     <row r="15" spans="1:20" s="27" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B15" s="23">
         <v>2017</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D15" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="L15" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="N15" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="O15" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="P15" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="E15" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="J15" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="K15" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="L15" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="M15" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="N15" s="52" t="s">
-        <v>79</v>
-      </c>
-      <c r="O15" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="P15" s="24" t="s">
-        <v>81</v>
-      </c>
       <c r="Q15" s="26" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="R15" s="47">
         <v>42904</v>
@@ -3003,113 +3000,113 @@
     </row>
     <row r="16" spans="1:20" s="27" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B16" s="23">
         <v>2017</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D16" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="L16" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="M16" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="N16" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="E16" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="24" t="s">
+      <c r="O16" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="G16" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="J16" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="K16" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="L16" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="M16" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="N16" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="O16" s="24" t="s">
-        <v>89</v>
-      </c>
       <c r="P16" s="24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q16" s="26" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="R16" s="26"/>
-      <c r="S16" s="59">
+      <c r="S16" s="58">
         <v>42952</v>
       </c>
       <c r="T16" s="48"/>
     </row>
     <row r="17" spans="1:20" s="27" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B17" s="23">
         <v>2017</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D17" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="L17" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="M17" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="N17" s="51" t="s">
+        <v>64</v>
+      </c>
+      <c r="O17" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="E17" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="H17" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="J17" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="K17" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="L17" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="M17" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="N17" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="O17" s="24" t="s">
-        <v>96</v>
-      </c>
       <c r="P17" s="24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q17" s="26" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="R17" s="47">
         <v>42902</v>
@@ -3121,55 +3118,55 @@
     </row>
     <row r="18" spans="1:20" s="27" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B18" s="23">
         <v>2017</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H18" s="24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J18" s="24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K18" s="24" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="L18" s="24" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="M18" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="N18" s="52" t="s">
-        <v>100</v>
+        <v>63</v>
+      </c>
+      <c r="N18" s="51" t="s">
+        <v>94</v>
       </c>
       <c r="O18" s="24" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="P18" s="24" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q18" s="26" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="R18" s="47">
         <v>42896</v>
@@ -3183,171 +3180,171 @@
     </row>
     <row r="19" spans="1:20" s="32" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B19" s="29">
         <v>2016</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F19" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G19" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H19" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I19" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J19" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K19" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L19" s="30" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="M19" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="N19" s="53" t="s">
-        <v>104</v>
+        <v>97</v>
+      </c>
+      <c r="N19" s="52" t="s">
+        <v>98</v>
       </c>
       <c r="O19" s="30" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="P19" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q19" s="31" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="R19" s="31"/>
-      <c r="S19" s="60">
+      <c r="S19" s="59">
         <v>42580</v>
       </c>
       <c r="T19" s="48"/>
     </row>
     <row r="20" spans="1:20" s="32" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B20" s="29">
         <v>2016</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F20" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H20" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I20" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J20" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K20" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L20" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M20" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="N20" s="53" t="s">
-        <v>106</v>
+        <v>7</v>
+      </c>
+      <c r="N20" s="52" t="s">
+        <v>100</v>
       </c>
       <c r="O20" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P20" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q20" s="31" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="R20" s="31"/>
-      <c r="S20" s="60">
+      <c r="S20" s="59">
         <v>42580</v>
       </c>
       <c r="T20" s="48"/>
     </row>
     <row r="21" spans="1:20" s="32" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B21" s="29">
         <v>2016</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F21" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G21" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H21" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I21" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J21" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K21" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L21" s="30" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="M21" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="N21" s="53" t="s">
-        <v>110</v>
+        <v>103</v>
+      </c>
+      <c r="N21" s="52" t="s">
+        <v>104</v>
       </c>
       <c r="O21" s="30" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="P21" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q21" s="31" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="R21" s="31"/>
       <c r="S21" s="31"/>
@@ -3355,55 +3352,55 @@
     </row>
     <row r="22" spans="1:20" s="32" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="28" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B22" s="29">
         <v>2016</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F22" s="30" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G22" s="30" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H22" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I22" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J22" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K22" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L22" s="30" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="M22" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="N22" s="53" t="s">
-        <v>117</v>
+        <v>110</v>
+      </c>
+      <c r="N22" s="52" t="s">
+        <v>111</v>
       </c>
       <c r="O22" s="30" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="P22" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q22" s="31" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="R22" s="31"/>
       <c r="S22" s="31"/>
@@ -3413,58 +3410,58 @@
     </row>
     <row r="23" spans="1:20" s="32" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="28" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B23" s="29">
         <v>2016</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G23" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H23" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I23" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J23" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K23" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L23" s="30" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="M23" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="N23" s="53" t="s">
-        <v>110</v>
+        <v>113</v>
+      </c>
+      <c r="N23" s="52" t="s">
+        <v>104</v>
       </c>
       <c r="O23" s="30" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="P23" s="30" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q23" s="31" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="R23" s="31"/>
-      <c r="S23" s="60">
+      <c r="S23" s="59">
         <v>42580</v>
       </c>
       <c r="T23" s="47">
@@ -3473,55 +3470,55 @@
     </row>
     <row r="24" spans="1:20" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="33" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B24" s="34">
         <v>2016</v>
       </c>
       <c r="C24" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E24" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F24" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G24" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H24" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I24" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J24" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K24" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L24" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M24" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="N24" s="54" t="s">
-        <v>123</v>
+        <v>116</v>
+      </c>
+      <c r="N24" s="53" t="s">
+        <v>117</v>
       </c>
       <c r="O24" s="35" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="P24" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q24" s="36" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="R24" s="36"/>
       <c r="S24" s="36"/>
@@ -3531,445 +3528,445 @@
     </row>
     <row r="25" spans="1:20" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="33" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B25" s="34">
         <v>2022</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D25" s="38"/>
       <c r="E25" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F25" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G25" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H25" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I25" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J25" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K25" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L25" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M25" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N25" s="54" t="s">
-        <v>128</v>
+        <v>7</v>
+      </c>
+      <c r="N25" s="53" t="s">
+        <v>122</v>
       </c>
       <c r="O25" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P25" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q25" s="39" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="R25" s="40"/>
-      <c r="S25" s="61">
+      <c r="S25" s="60">
         <v>44743</v>
       </c>
       <c r="T25" s="48"/>
     </row>
     <row r="26" spans="1:20" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="33" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B26" s="34">
         <v>2022</v>
       </c>
       <c r="C26" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D26" s="38"/>
       <c r="E26" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F26" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G26" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H26" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I26" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J26" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K26" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L26" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M26" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N26" s="55" t="s">
-        <v>141</v>
+        <v>7</v>
+      </c>
+      <c r="N26" s="54" t="s">
+        <v>135</v>
       </c>
       <c r="O26" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P26" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q26" s="39" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="R26" s="40"/>
-      <c r="S26" s="61">
+      <c r="S26" s="60">
         <v>44743</v>
       </c>
       <c r="T26" s="48"/>
     </row>
     <row r="27" spans="1:20" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="33" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B27" s="34">
         <v>2022</v>
       </c>
       <c r="C27" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D27" s="38"/>
       <c r="E27" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F27" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G27" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H27" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I27" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J27" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K27" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L27" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M27" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N27" s="54" t="s">
-        <v>129</v>
+        <v>7</v>
+      </c>
+      <c r="N27" s="53" t="s">
+        <v>123</v>
       </c>
       <c r="O27" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P27" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q27" s="41" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="R27" s="40"/>
-      <c r="S27" s="61">
+      <c r="S27" s="60">
         <v>44743</v>
       </c>
       <c r="T27" s="48"/>
     </row>
     <row r="28" spans="1:20" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="33" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B28" s="34">
         <v>2022</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D28" s="38"/>
       <c r="E28" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F28" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G28" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H28" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I28" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J28" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K28" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L28" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M28" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N28" s="54" t="s">
-        <v>131</v>
+        <v>7</v>
+      </c>
+      <c r="N28" s="53" t="s">
+        <v>125</v>
       </c>
       <c r="O28" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P28" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q28" s="41" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="R28" s="40"/>
-      <c r="S28" s="61">
+      <c r="S28" s="60">
         <v>44743</v>
       </c>
       <c r="T28" s="48"/>
     </row>
     <row r="29" spans="1:20" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="33" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B29" s="34">
         <v>2022</v>
       </c>
       <c r="C29" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D29" s="38"/>
       <c r="E29" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F29" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G29" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H29" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I29" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J29" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K29" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L29" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M29" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N29" s="54" t="s">
-        <v>126</v>
+        <v>7</v>
+      </c>
+      <c r="N29" s="53" t="s">
+        <v>120</v>
       </c>
       <c r="O29" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P29" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q29" s="39" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="R29" s="40"/>
-      <c r="S29" s="61">
+      <c r="S29" s="60">
         <v>44773</v>
       </c>
       <c r="T29" s="48"/>
     </row>
     <row r="30" spans="1:20" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="33" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B30" s="34">
         <v>2022</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D30" s="38"/>
       <c r="E30" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F30" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G30" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H30" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I30" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J30" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K30" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L30" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M30" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N30" s="54" t="s">
-        <v>132</v>
+        <v>7</v>
+      </c>
+      <c r="N30" s="53" t="s">
+        <v>126</v>
       </c>
       <c r="O30" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P30" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q30" s="41" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="R30" s="40"/>
-      <c r="S30" s="61">
+      <c r="S30" s="60">
         <v>44762</v>
       </c>
       <c r="T30" s="48"/>
     </row>
     <row r="31" spans="1:20" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="33" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B31" s="34">
         <v>2022</v>
       </c>
       <c r="C31" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D31" s="38"/>
       <c r="E31" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F31" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G31" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H31" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I31" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J31" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K31" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L31" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M31" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N31" s="54" t="s">
-        <v>134</v>
+        <v>7</v>
+      </c>
+      <c r="N31" s="53" t="s">
+        <v>128</v>
       </c>
       <c r="O31" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P31" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q31" s="41" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="R31" s="40"/>
-      <c r="S31" s="61">
+      <c r="S31" s="60">
         <v>44770</v>
       </c>
       <c r="T31" s="48"/>
     </row>
     <row r="32" spans="1:20" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="33" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B32" s="34">
         <v>2022</v>
       </c>
       <c r="C32" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D32" s="38"/>
       <c r="E32" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F32" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G32" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H32" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I32" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J32" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K32" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L32" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M32" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N32" s="54" t="s">
-        <v>125</v>
+        <v>7</v>
+      </c>
+      <c r="N32" s="53" t="s">
+        <v>119</v>
       </c>
       <c r="O32" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P32" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q32" s="41" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="R32" s="40"/>
       <c r="S32" s="40"/>
@@ -3977,165 +3974,165 @@
     </row>
     <row r="33" spans="1:50" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="33" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B33" s="34">
         <v>2022</v>
       </c>
       <c r="C33" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D33" s="38"/>
       <c r="E33" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F33" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G33" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H33" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I33" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J33" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K33" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L33" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M33" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N33" s="54" t="s">
-        <v>137</v>
+        <v>7</v>
+      </c>
+      <c r="N33" s="53" t="s">
+        <v>131</v>
       </c>
       <c r="O33" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P33" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q33" s="41" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="R33" s="40"/>
-      <c r="S33" s="61">
+      <c r="S33" s="60">
         <v>44764</v>
       </c>
       <c r="T33" s="48"/>
     </row>
     <row r="34" spans="1:50" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="33" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B34" s="34">
         <v>2022</v>
       </c>
       <c r="C34" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D34" s="38"/>
       <c r="E34" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F34" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G34" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H34" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I34" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J34" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K34" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L34" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M34" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N34" s="54" t="s">
-        <v>139</v>
+        <v>7</v>
+      </c>
+      <c r="N34" s="53" t="s">
+        <v>133</v>
       </c>
       <c r="O34" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P34" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q34" s="39" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="R34" s="40"/>
-      <c r="S34" s="62">
+      <c r="S34" s="61">
         <v>44768</v>
       </c>
       <c r="T34" s="48"/>
     </row>
     <row r="35" spans="1:50" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="33" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B35" s="34">
         <v>2022</v>
       </c>
       <c r="C35" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D35" s="38"/>
       <c r="E35" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F35" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G35" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H35" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I35" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J35" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K35" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L35" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M35" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N35" s="54" t="s">
-        <v>141</v>
+        <v>7</v>
+      </c>
+      <c r="N35" s="53" t="s">
+        <v>135</v>
       </c>
       <c r="O35" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P35" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q35" s="41" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="R35" s="40"/>
       <c r="S35" s="40"/>
@@ -4143,391 +4140,391 @@
     </row>
     <row r="36" spans="1:50" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="33" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B36" s="34">
         <v>2022</v>
       </c>
       <c r="C36" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D36" s="38"/>
       <c r="E36" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F36" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G36" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H36" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I36" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J36" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K36" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L36" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M36" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N36" s="54" t="s">
-        <v>134</v>
+        <v>7</v>
+      </c>
+      <c r="N36" s="53" t="s">
+        <v>128</v>
       </c>
       <c r="O36" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P36" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q36" s="41" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="R36" s="40"/>
-      <c r="S36" s="62">
+      <c r="S36" s="61">
         <v>44769</v>
       </c>
       <c r="T36" s="48"/>
     </row>
     <row r="37" spans="1:50" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="33" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B37" s="34">
         <v>2022</v>
       </c>
       <c r="C37" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D37" s="38"/>
       <c r="E37" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F37" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G37" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H37" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I37" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J37" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K37" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L37" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M37" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N37" s="54" t="s">
-        <v>144</v>
+        <v>7</v>
+      </c>
+      <c r="N37" s="53" t="s">
+        <v>138</v>
       </c>
       <c r="O37" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P37" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q37" s="39" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="R37" s="40"/>
-      <c r="S37" s="61">
+      <c r="S37" s="60">
         <v>44776</v>
       </c>
       <c r="T37" s="48"/>
     </row>
     <row r="38" spans="1:50" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="33" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B38" s="34">
         <v>2022</v>
       </c>
       <c r="C38" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D38" s="38"/>
       <c r="E38" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F38" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G38" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H38" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I38" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J38" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K38" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L38" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M38" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N38" s="54" t="s">
-        <v>145</v>
+        <v>7</v>
+      </c>
+      <c r="N38" s="53" t="s">
+        <v>139</v>
       </c>
       <c r="O38" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P38" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q38" s="41" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="R38" s="40"/>
-      <c r="S38" s="61">
+      <c r="S38" s="60">
         <v>44771</v>
       </c>
       <c r="T38" s="48"/>
     </row>
     <row r="39" spans="1:50" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="33" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B39" s="34">
         <v>2022</v>
       </c>
       <c r="C39" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D39" s="38"/>
       <c r="E39" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F39" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G39" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H39" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I39" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J39" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K39" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L39" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M39" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N39" s="54" t="s">
-        <v>126</v>
+        <v>7</v>
+      </c>
+      <c r="N39" s="53" t="s">
+        <v>120</v>
       </c>
       <c r="O39" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P39" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q39" s="41" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="R39" s="40"/>
-      <c r="S39" s="61">
+      <c r="S39" s="60">
         <v>44776</v>
       </c>
       <c r="T39" s="48"/>
     </row>
     <row r="40" spans="1:50" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="33" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B40" s="34">
         <v>2022</v>
       </c>
       <c r="C40" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D40" s="38"/>
       <c r="E40" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F40" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G40" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H40" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I40" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J40" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K40" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L40" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M40" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N40" s="54" t="s">
-        <v>127</v>
+        <v>7</v>
+      </c>
+      <c r="N40" s="53" t="s">
+        <v>121</v>
       </c>
       <c r="O40" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P40" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q40" s="41" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="R40" s="40"/>
-      <c r="S40" s="61">
+      <c r="S40" s="60">
         <v>44778</v>
       </c>
       <c r="T40" s="48"/>
     </row>
     <row r="41" spans="1:50" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="33" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B41" s="34">
         <v>2022</v>
       </c>
       <c r="C41" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D41" s="38"/>
       <c r="E41" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F41" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G41" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H41" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I41" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J41" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K41" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L41" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M41" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N41" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="N41" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="O41" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="P41" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q41" s="41" t="s">
         <v>149</v>
       </c>
-      <c r="O41" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="P41" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q41" s="41" t="s">
-        <v>155</v>
-      </c>
       <c r="R41" s="40"/>
-      <c r="S41" s="61">
+      <c r="S41" s="60">
         <v>44771</v>
       </c>
       <c r="T41" s="48"/>
     </row>
     <row r="42" spans="1:50" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="33" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B42" s="36">
         <v>2022</v>
       </c>
       <c r="C42" s="36" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E42" s="41" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F42" s="41" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G42" s="41" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H42" s="41" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I42" s="41" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J42" s="41" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K42" s="41" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L42" s="41" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M42" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="N42" s="56" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="N42" s="55" t="s">
+        <v>7</v>
       </c>
       <c r="O42" s="41" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P42" s="41" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q42" s="39" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="R42" s="40"/>
-      <c r="S42" s="62">
+      <c r="S42" s="61">
         <v>44769</v>
       </c>
       <c r="T42" s="48"/>
@@ -4564,116 +4561,116 @@
     </row>
     <row r="43" spans="1:50" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="33" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B43" s="34">
         <v>2022</v>
       </c>
       <c r="C43" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D43" s="38"/>
       <c r="E43" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F43" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G43" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H43" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I43" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J43" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K43" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L43" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M43" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N43" s="54" t="s">
-        <v>134</v>
+        <v>7</v>
+      </c>
+      <c r="N43" s="53" t="s">
+        <v>128</v>
       </c>
       <c r="O43" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P43" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q43" s="39" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="R43" s="40"/>
-      <c r="S43" s="62">
+      <c r="S43" s="61">
         <v>44773</v>
       </c>
       <c r="T43" s="48"/>
     </row>
     <row r="44" spans="1:50" s="37" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="33" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B44" s="34">
         <v>2022</v>
       </c>
       <c r="C44" s="35" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D44" s="38"/>
       <c r="E44" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F44" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G44" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H44" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I44" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J44" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="K44" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L44" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M44" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N44" s="54" t="s">
-        <v>141</v>
+        <v>7</v>
+      </c>
+      <c r="N44" s="53" t="s">
+        <v>135</v>
       </c>
       <c r="O44" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P44" s="35" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q44" s="39" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="R44" s="40"/>
       <c r="S44" s="40"/>
       <c r="T44" s="40"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="V42 X42 Z42 AB42 AD42 AF42 AH42">
+  <conditionalFormatting sqref="X42 V42 Z42 AB42 AD42 AF42 AH42">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="formula" val="1"/>

</xml_diff>